<commit_message>
fixed error in heval4
</commit_message>
<xml_diff>
--- a/data/processed/4th/MASTER_combined_4th.xlsx
+++ b/data/processed/4th/MASTER_combined_4th.xlsx
@@ -9939,7 +9939,7 @@
       </c>
       <c r="T119"/>
       <c r="U119" t="s">
-        <v>47</v>
+        <v>90</v>
       </c>
     </row>
     <row r="120">
@@ -10002,7 +10002,7 @@
       </c>
       <c r="T120"/>
       <c r="U120" t="s">
-        <v>73</v>
+        <v>115</v>
       </c>
     </row>
     <row r="121">
@@ -10065,7 +10065,7 @@
       </c>
       <c r="T121"/>
       <c r="U121" t="s">
-        <v>90</v>
+        <v>127</v>
       </c>
     </row>
     <row r="122">
@@ -10130,7 +10130,7 @@
         <v>144</v>
       </c>
       <c r="U122" t="s">
-        <v>102</v>
+        <v>73</v>
       </c>
     </row>
     <row r="123">
@@ -10193,7 +10193,7 @@
       </c>
       <c r="T123"/>
       <c r="U123" t="s">
-        <v>115</v>
+        <v>128</v>
       </c>
     </row>
     <row r="124">
@@ -10256,7 +10256,7 @@
       </c>
       <c r="T124"/>
       <c r="U124" t="s">
-        <v>127</v>
+        <v>102</v>
       </c>
     </row>
     <row r="125">
@@ -10321,7 +10321,7 @@
         <v>145</v>
       </c>
       <c r="U125" t="s">
-        <v>128</v>
+        <v>53</v>
       </c>
     </row>
     <row r="126">
@@ -10892,7 +10892,7 @@
       </c>
       <c r="T134"/>
       <c r="U134" t="s">
-        <v>90</v>
+        <v>127</v>
       </c>
     </row>
     <row r="135">
@@ -11083,7 +11083,7 @@
         <v>151</v>
       </c>
       <c r="U137" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
     </row>
     <row r="138">
@@ -11148,7 +11148,7 @@
         <v>152</v>
       </c>
       <c r="U138" t="s">
-        <v>102</v>
+        <v>73</v>
       </c>
     </row>
     <row r="139">
@@ -11274,7 +11274,7 @@
       </c>
       <c r="T140"/>
       <c r="U140" t="s">
-        <v>73</v>
+        <v>115</v>
       </c>
     </row>
     <row r="141">

</xml_diff>